<commit_message>
IE update to include categories
</commit_message>
<xml_diff>
--- a/curation/draft/collection/collection_specialization_IE.xlsx
+++ b/curation/draft/collection/collection_specialization_IE.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\collection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dagmarkottig/COSMoS/curation/draft/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556EACC6-507C-40AF-8E1A-90DCAB30E9B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F43BB9-4E99-434F-9761-5E839E48470F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4300" yWindow="780" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Collection_IE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_IE!$A$1:$AG$17</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Collection_IE!$A$1:$AH$17</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="89">
   <si>
     <t>package_date</t>
   </si>
@@ -280,9 +280,6 @@
     <t>EXCL01;EXCL02;EXCL03; EXCL04;EXCL05;EXCL06; EXCL07;EXCL08; EXCL09;EXCL10;EXCL11;EXCL12;EXCL13;EXCL14;EXCL15;EXCL16;EXCL17;EXCL18;EXCL19;EXCL20;EXCL21;EXCL22;EXCL23;EXCL24;EXCL25</t>
   </si>
   <si>
-    <t>360i</t>
-  </si>
-  <si>
     <t>Without Date</t>
   </si>
   <si>
@@ -290,6 +287,9 @@
   </si>
   <si>
     <t>EXCL01_SHORT_360</t>
+  </si>
+  <si>
+    <t>categories</t>
   </si>
 </sst>
 </file>
@@ -693,40 +693,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG17"/>
+  <dimension ref="A1:AH17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="5"/>
-    <col min="8" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" customWidth="1"/>
-    <col min="15" max="15" width="31.85546875" style="3" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" customWidth="1"/>
-    <col min="24" max="24" width="19.85546875" customWidth="1"/>
-    <col min="25" max="25" width="20.28515625" style="3" customWidth="1"/>
-    <col min="26" max="26" width="19.42578125" style="3" customWidth="1"/>
-    <col min="27" max="27" width="14.28515625" customWidth="1"/>
-    <col min="28" max="28" width="21.28515625" customWidth="1"/>
-    <col min="30" max="30" width="17.42578125" customWidth="1"/>
-    <col min="31" max="31" width="16" style="3" customWidth="1"/>
-    <col min="32" max="32" width="15.28515625" customWidth="1"/>
-    <col min="33" max="33" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="5"/>
+    <col min="8" max="8" width="21.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" customWidth="1"/>
+    <col min="10" max="11" width="12.83203125" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" customWidth="1"/>
+    <col min="16" max="16" width="31.83203125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" customWidth="1"/>
+    <col min="19" max="19" width="17.5" customWidth="1"/>
+    <col min="22" max="22" width="15.1640625" customWidth="1"/>
+    <col min="23" max="23" width="10.83203125" customWidth="1"/>
+    <col min="25" max="25" width="19.83203125" customWidth="1"/>
+    <col min="26" max="26" width="20.33203125" style="3" customWidth="1"/>
+    <col min="27" max="27" width="19.5" style="3" customWidth="1"/>
+    <col min="28" max="28" width="14.33203125" customWidth="1"/>
+    <col min="29" max="29" width="21.33203125" customWidth="1"/>
+    <col min="31" max="31" width="17.5" customWidth="1"/>
+    <col min="32" max="32" width="16" style="3" customWidth="1"/>
+    <col min="33" max="33" width="15.33203125" customWidth="1"/>
+    <col min="34" max="34" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,76 +758,79 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="48" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>62</v>
       </c>
@@ -843,56 +846,56 @@
       <c r="H2" t="s">
         <v>63</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="L2" t="s">
-        <v>33</v>
       </c>
       <c r="M2" t="s">
         <v>33</v>
       </c>
       <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
         <v>62</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>1</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>45</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>36</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>1</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>48</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>77</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>78</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>51</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="48" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>62</v>
       </c>
@@ -908,44 +911,44 @@
       <c r="H3" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="L3" t="s">
-        <v>37</v>
       </c>
       <c r="M3" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>2</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>48</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>39</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>10</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>48</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>40</v>
       </c>
       <c r="AE3" t="s">
         <v>40</v>
       </c>
+      <c r="AF3" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="4" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>41</v>
       </c>
@@ -964,44 +967,44 @@
       <c r="H4" t="s">
         <v>75</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="L4" t="s">
-        <v>37</v>
       </c>
       <c r="M4" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>1</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>45</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>39</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>10</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>48</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>40</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>41</v>
       </c>
@@ -1020,56 +1023,56 @@
       <c r="H5" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="L5" t="s">
-        <v>42</v>
-      </c>
       <c r="M5" t="s">
         <v>42</v>
       </c>
       <c r="N5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O5" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>2</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>45</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>36</v>
       </c>
-      <c r="T5">
+      <c r="U5">
         <v>15</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>48</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>46</v>
       </c>
-      <c r="X5" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB5" t="s">
+      <c r="Y5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC5" t="s">
         <v>47</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>41</v>
       </c>
-      <c r="AD5" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE5" s="3" t="s">
+      <c r="AE5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF5" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>41</v>
       </c>
@@ -1088,53 +1091,53 @@
       <c r="H6" t="s">
         <v>75</v>
       </c>
-      <c r="K6" s="6" t="s">
+      <c r="L6" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="L6" t="s">
-        <v>73</v>
       </c>
       <c r="M6" t="s">
         <v>73</v>
       </c>
       <c r="N6" t="s">
+        <v>73</v>
+      </c>
+      <c r="O6" t="s">
         <v>72</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>3</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>45</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>36</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>20</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>48</v>
-      </c>
-      <c r="Y6" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AA6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB6" t="s">
         <v>52</v>
       </c>
-      <c r="AD6" s="3" t="s">
+      <c r="AE6" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AE6" s="3" t="s">
+      <c r="AF6" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>58</v>
       </c>
@@ -1153,44 +1156,44 @@
       <c r="H7" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="L7" t="s">
-        <v>37</v>
       </c>
       <c r="M7" t="s">
         <v>37</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="N7" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="P7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>1</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>45</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>39</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>10</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>48</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>40</v>
       </c>
-      <c r="AE7" s="3" t="s">
+      <c r="AF7" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>58</v>
       </c>
@@ -1209,56 +1212,56 @@
       <c r="H8" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="L8" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="L8" t="s">
-        <v>42</v>
-      </c>
       <c r="M8" t="s">
         <v>42</v>
       </c>
       <c r="N8" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" t="s">
         <v>43</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="P8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>2</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>45</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>36</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>15</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>48</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>46</v>
       </c>
-      <c r="X8" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB8" t="s">
+      <c r="Y8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC8" t="s">
         <v>56</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>58</v>
       </c>
-      <c r="AD8" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE8" s="3" t="s">
+      <c r="AE8" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF8" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>58</v>
       </c>
@@ -1277,53 +1280,53 @@
       <c r="H9" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="L9" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="L9" t="s">
-        <v>73</v>
       </c>
       <c r="M9" t="s">
         <v>73</v>
       </c>
       <c r="N9" t="s">
+        <v>73</v>
+      </c>
+      <c r="O9" t="s">
         <v>72</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="P9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>3</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>45</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>36</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>20</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>48</v>
-      </c>
-      <c r="Y9" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="Z9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AA9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB9" t="s">
         <v>52</v>
       </c>
-      <c r="AD9" s="3" t="s">
+      <c r="AE9" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AE9" s="3" t="s">
+      <c r="AF9" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>41</v>
       </c>
@@ -1343,58 +1346,58 @@
         <v>81</v>
       </c>
       <c r="J10" t="s">
-        <v>86</v>
-      </c>
-      <c r="K10" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="L10" t="s">
-        <v>42</v>
-      </c>
       <c r="M10" t="s">
         <v>42</v>
       </c>
       <c r="N10" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" t="s">
         <v>43</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="P10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>2</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>45</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>36</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>15</v>
       </c>
-      <c r="V10" t="s">
+      <c r="W10" t="s">
         <v>48</v>
       </c>
-      <c r="W10" t="s">
+      <c r="X10" t="s">
         <v>46</v>
       </c>
-      <c r="X10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB10" t="s">
+      <c r="Y10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC10" t="s">
         <v>47</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>41</v>
       </c>
-      <c r="AD10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE10" s="3" t="s">
+      <c r="AE10" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF10" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>41</v>
       </c>
@@ -1414,55 +1417,55 @@
         <v>81</v>
       </c>
       <c r="J11" t="s">
-        <v>86</v>
-      </c>
-      <c r="K11" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="L11" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="L11" t="s">
-        <v>73</v>
       </c>
       <c r="M11" t="s">
         <v>73</v>
       </c>
       <c r="N11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O11" t="s">
         <v>72</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="P11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>3</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>45</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>36</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>20</v>
       </c>
-      <c r="V11" t="s">
+      <c r="W11" t="s">
         <v>48</v>
-      </c>
-      <c r="Y11" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="Z11" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AA11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB11" t="s">
         <v>52</v>
       </c>
-      <c r="AD11" s="3" t="s">
+      <c r="AE11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AE11" s="3" t="s">
+      <c r="AF11" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>58</v>
       </c>
@@ -1482,58 +1485,58 @@
         <v>82</v>
       </c>
       <c r="J12" t="s">
-        <v>86</v>
-      </c>
-      <c r="K12" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="L12" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="L12" t="s">
-        <v>42</v>
-      </c>
       <c r="M12" t="s">
         <v>42</v>
       </c>
       <c r="N12" t="s">
+        <v>42</v>
+      </c>
+      <c r="O12" t="s">
         <v>43</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="P12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>2</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>45</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>36</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>15</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>48</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>46</v>
       </c>
-      <c r="X12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB12" t="s">
+      <c r="Y12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC12" t="s">
         <v>56</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>58</v>
       </c>
-      <c r="AD12" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE12" s="3" t="s">
+      <c r="AE12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF12" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>58</v>
       </c>
@@ -1553,55 +1556,55 @@
         <v>82</v>
       </c>
       <c r="J13" t="s">
-        <v>86</v>
-      </c>
-      <c r="K13" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="L13" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="L13" t="s">
-        <v>73</v>
       </c>
       <c r="M13" t="s">
         <v>73</v>
       </c>
       <c r="N13" t="s">
+        <v>73</v>
+      </c>
+      <c r="O13" t="s">
         <v>72</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="P13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>3</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>45</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>36</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>20</v>
       </c>
-      <c r="V13" t="s">
+      <c r="W13" t="s">
         <v>48</v>
-      </c>
-      <c r="Y13" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="Z13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AA13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB13" t="s">
         <v>52</v>
       </c>
-      <c r="AD13" s="3" t="s">
+      <c r="AE13" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AE13" s="3" t="s">
+      <c r="AF13" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>41</v>
       </c>
@@ -1618,61 +1621,61 @@
         <v>32</v>
       </c>
       <c r="H14" t="s">
-        <v>87</v>
-      </c>
-      <c r="J14" t="s">
-        <v>85</v>
-      </c>
-      <c r="K14" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K14">
+        <v>360</v>
+      </c>
+      <c r="L14" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="L14" t="s">
-        <v>42</v>
-      </c>
       <c r="M14" t="s">
         <v>42</v>
       </c>
       <c r="N14" t="s">
+        <v>42</v>
+      </c>
+      <c r="O14" t="s">
         <v>43</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="P14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>2</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>45</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>36</v>
       </c>
-      <c r="T14">
+      <c r="U14">
         <v>15</v>
       </c>
-      <c r="V14" t="s">
+      <c r="W14" t="s">
         <v>48</v>
       </c>
-      <c r="W14" t="s">
+      <c r="X14" t="s">
         <v>46</v>
       </c>
-      <c r="X14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB14" t="s">
+      <c r="Y14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC14" t="s">
         <v>47</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AD14" t="s">
         <v>41</v>
       </c>
-      <c r="AD14" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE14" s="3" t="s">
+      <c r="AE14" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF14" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:33" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="48" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>41</v>
       </c>
@@ -1689,58 +1692,58 @@
         <v>32</v>
       </c>
       <c r="H15" t="s">
-        <v>87</v>
-      </c>
-      <c r="J15" t="s">
-        <v>85</v>
-      </c>
-      <c r="K15" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K15">
+        <v>360</v>
+      </c>
+      <c r="L15" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="L15" t="s">
-        <v>73</v>
       </c>
       <c r="M15" t="s">
         <v>73</v>
       </c>
       <c r="N15" t="s">
+        <v>73</v>
+      </c>
+      <c r="O15" t="s">
         <v>72</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="P15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>3</v>
       </c>
-      <c r="R15" t="s">
+      <c r="S15" t="s">
         <v>45</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>36</v>
       </c>
-      <c r="T15">
+      <c r="U15">
         <v>20</v>
       </c>
-      <c r="V15" t="s">
+      <c r="W15" t="s">
         <v>48</v>
-      </c>
-      <c r="Y15" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="Z15" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="AA15" t="s">
+      <c r="AA15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB15" t="s">
         <v>52</v>
       </c>
-      <c r="AD15" s="3" t="s">
+      <c r="AE15" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AE15" s="3" t="s">
+      <c r="AF15" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>58</v>
       </c>
@@ -1757,61 +1760,61 @@
         <v>32</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="J16" t="s">
-        <v>85</v>
-      </c>
-      <c r="K16" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K16">
+        <v>360</v>
+      </c>
+      <c r="L16" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="L16" t="s">
-        <v>42</v>
-      </c>
       <c r="M16" t="s">
         <v>42</v>
       </c>
       <c r="N16" t="s">
+        <v>42</v>
+      </c>
+      <c r="O16" t="s">
         <v>43</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="P16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>2</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>45</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>36</v>
       </c>
-      <c r="T16">
+      <c r="U16">
         <v>15</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>48</v>
       </c>
-      <c r="W16" t="s">
+      <c r="X16" t="s">
         <v>46</v>
       </c>
-      <c r="X16" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB16" t="s">
+      <c r="Y16" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC16" t="s">
         <v>56</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="AD16" t="s">
         <v>58</v>
       </c>
-      <c r="AD16" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE16" s="3" t="s">
+      <c r="AE16" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF16" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="2:31" ht="165" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:32" ht="160" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>58</v>
       </c>
@@ -1828,70 +1831,70 @@
         <v>32</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="J17" t="s">
-        <v>85</v>
-      </c>
-      <c r="K17" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K17">
+        <v>360</v>
+      </c>
+      <c r="L17" s="6" t="s">
         <v>80</v>
-      </c>
-      <c r="L17" t="s">
-        <v>73</v>
       </c>
       <c r="M17" t="s">
         <v>73</v>
       </c>
       <c r="N17" t="s">
+        <v>73</v>
+      </c>
+      <c r="O17" t="s">
         <v>72</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="P17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>3</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>45</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>36</v>
       </c>
-      <c r="T17">
+      <c r="U17">
         <v>20</v>
       </c>
-      <c r="V17" t="s">
+      <c r="W17" t="s">
         <v>48</v>
-      </c>
-      <c r="Y17" s="3" t="s">
-        <v>84</v>
       </c>
       <c r="Z17" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="AA17" t="s">
+      <c r="AA17" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB17" t="s">
         <v>52</v>
       </c>
-      <c r="AD17" s="3" t="s">
+      <c r="AE17" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AE17" s="3" t="s">
+      <c r="AF17" s="3" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AH17" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="N8" r:id="rId1" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25372" xr:uid="{9B61766A-B66B-EC4E-9724-1F0A521D88FB}"/>
-    <hyperlink ref="N6" r:id="rId2" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C181043" xr:uid="{5F41BA7F-79FA-9742-A3E9-D89D1C7591A0}"/>
-    <hyperlink ref="N9" r:id="rId3" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C181043" xr:uid="{7509BA1E-4AC1-5045-A19B-CD30E6ED6532}"/>
-    <hyperlink ref="N12" r:id="rId4" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25372" xr:uid="{1D7312B8-9B3D-6843-955D-5F738BD9AD83}"/>
-    <hyperlink ref="N11" r:id="rId5" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C181043" xr:uid="{A39A3100-940D-894D-AF2C-2BD9AD5ABAD5}"/>
-    <hyperlink ref="N13" r:id="rId6" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C181043" xr:uid="{E5F45EB2-3D25-1E41-9C4F-6D66759EA74B}"/>
-    <hyperlink ref="N16" r:id="rId7" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25372" xr:uid="{06AA3567-10B4-4F4E-8F0D-3C1765659FA6}"/>
-    <hyperlink ref="N15" r:id="rId8" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C181043" xr:uid="{41372C07-559B-EC48-A143-FF05A4732DF8}"/>
-    <hyperlink ref="N17" r:id="rId9" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C181043" xr:uid="{F02C1199-BA40-F64E-A623-6CBB91AB665C}"/>
+    <hyperlink ref="O8" r:id="rId1" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25372" xr:uid="{9B61766A-B66B-EC4E-9724-1F0A521D88FB}"/>
+    <hyperlink ref="O6" r:id="rId2" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C181043" xr:uid="{5F41BA7F-79FA-9742-A3E9-D89D1C7591A0}"/>
+    <hyperlink ref="O9" r:id="rId3" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C181043" xr:uid="{7509BA1E-4AC1-5045-A19B-CD30E6ED6532}"/>
+    <hyperlink ref="O12" r:id="rId4" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25372" xr:uid="{1D7312B8-9B3D-6843-955D-5F738BD9AD83}"/>
+    <hyperlink ref="O11" r:id="rId5" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C181043" xr:uid="{A39A3100-940D-894D-AF2C-2BD9AD5ABAD5}"/>
+    <hyperlink ref="O13" r:id="rId6" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C181043" xr:uid="{E5F45EB2-3D25-1E41-9C4F-6D66759EA74B}"/>
+    <hyperlink ref="O16" r:id="rId7" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25372" xr:uid="{06AA3567-10B4-4F4E-8F0D-3C1765659FA6}"/>
+    <hyperlink ref="O15" r:id="rId8" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C181043" xr:uid="{41372C07-559B-EC48-A143-FF05A4732DF8}"/>
+    <hyperlink ref="O17" r:id="rId9" display="https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C181043" xr:uid="{F02C1199-BA40-F64E-A623-6CBB91AB665C}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId10"/>

</xml_diff>